<commit_message>
tr: jp credit addition
</commit_message>
<xml_diff>
--- a/ExtremeRolesTransData.xlsx
+++ b/ExtremeRolesTransData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\.PROJ\GIT\ExtremeRoles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9371AFB-7F6E-49A0-964B-457BB784AA16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9426FE48-3AAF-48B8-ADF0-53A2995D0F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="4335" windowWidth="20910" windowHeight="11835" tabRatio="500" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2265" yWindow="975" windowWidth="26160" windowHeight="11835" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7341" uniqueCount="5375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7343" uniqueCount="5377">
   <si>
     <t>English</t>
   </si>
@@ -24920,6 +24920,20 @@
 このシールドはヴィランによるキルや、自爆等の特殊キルには効果がない。
 &lt;/indent&gt;
 &lt;br&gt;</t>
+    <phoneticPr fontId="31"/>
+  </si>
+  <si>
+    <t>文章（テスト中）：</t>
+    <rPh sb="0" eb="2">
+      <t>ブンショウ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>チュウ</t>
+    </rPh>
+    <phoneticPr fontId="31"/>
+  </si>
+  <si>
+    <t>Yuhgao</t>
     <phoneticPr fontId="31"/>
   </si>
 </sst>
@@ -26260,8 +26274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q334"/>
   <sheetViews>
-    <sheetView topLeftCell="A140" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" topLeftCell="A327" workbookViewId="0">
+      <selection activeCell="M339" sqref="M339"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -27431,6 +27445,9 @@
       <c r="B94" s="3" t="s">
         <v>325</v>
       </c>
+      <c r="M94" t="s">
+        <v>5375</v>
+      </c>
       <c r="O94" t="s">
         <v>326</v>
       </c>
@@ -27441,6 +27458,9 @@
       </c>
       <c r="B95" s="3" t="s">
         <v>328</v>
+      </c>
+      <c r="M95" t="s">
+        <v>5376</v>
       </c>
       <c r="O95" t="s">
         <v>329</v>
@@ -50750,7 +50770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J2" workbookViewId="0">
+    <sheetView topLeftCell="J2" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>

</xml_diff>